<commit_message>
added random state comparison, generated venn diagrams for testing set overlap. nearing finalization on manuscript
</commit_message>
<xml_diff>
--- a/score_based/SGD/metric_comparisons_between_k_values.xlsx
+++ b/score_based/SGD/metric_comparisons_between_k_values.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livememphis-my.sharepoint.com/personal/gszwbwsk_memphis_edu/Documents/Machine Learning/ph4_classification/score_based/SGD/clustering_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livememphis-my.sharepoint.com/personal/gszwbwsk_memphis_edu/Documents/Machine Learning/ph4_classification/score_based/SGD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22C66F47-F0F9-431B-964C-7E60EE08A0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{22C66F47-F0F9-431B-964C-7E60EE08A0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B05256CB-ADDD-4931-9842-63B16DBEC716}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7B000C7F-98D0-46A4-AB29-B05331BD6BDF}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="28800" windowHeight="9120" xr2:uid="{7B000C7F-98D0-46A4-AB29-B05331BD6BDF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="randomstate = 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -218,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -229,8 +229,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -546,23 +544,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD22F84-DFA3-47F7-972A-93D40CCA3052}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="A2:G8"/>
+      <selection activeCell="B26" sqref="B26:F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -585,7 +583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -614,7 +612,7 @@
         <v>0.88250000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -640,14 +638,14 @@
         <v>0.6825</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="7"/>
       <c r="D5">
-        <f t="shared" ref="D4:D5" si="3">AVERAGE(C17:F17)</f>
+        <f t="shared" ref="D5" si="3">AVERAGE(C17:F17)</f>
         <v>0.64750000000000008</v>
       </c>
       <c r="E5">
@@ -663,7 +661,7 @@
         <v>0.85749999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -683,7 +681,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -700,7 +698,7 @@
         <v>0.88750000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -709,12 +707,12 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="12">
+      <c r="G8" s="10">
         <f t="shared" si="2"/>
         <v>0.1125</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -734,11 +732,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
@@ -754,7 +752,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -774,7 +772,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -794,8 +792,8 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15">
@@ -814,8 +812,8 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16">
@@ -834,8 +832,8 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17">
@@ -854,8 +852,8 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>2</v>
       </c>
       <c r="B18">
@@ -874,8 +872,8 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19">
@@ -894,8 +892,8 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>4</v>
       </c>
       <c r="B20">
@@ -914,8 +912,8 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21">
@@ -934,8 +932,8 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>2</v>
       </c>
       <c r="B22">
@@ -954,8 +952,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>3</v>
       </c>
       <c r="B23">
@@ -974,8 +972,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24">
@@ -994,8 +992,8 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25">
@@ -1014,8 +1012,8 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>6</v>
       </c>
       <c r="B26">
@@ -1034,8 +1032,8 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>2</v>
       </c>
       <c r="B27">
@@ -1054,8 +1052,8 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>3</v>
       </c>
       <c r="B28">
@@ -1074,8 +1072,8 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="11" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>4</v>
       </c>
       <c r="B29">
@@ -1094,8 +1092,8 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="11" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30">
@@ -1114,8 +1112,8 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="11" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>6</v>
       </c>
       <c r="B31">
@@ -1134,8 +1132,8 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="11" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>7</v>
       </c>
       <c r="B32">
@@ -1153,9 +1151,6 @@
       <c r="F32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>